<commit_message>
Updated all APIs (except auth) for the new DB schema
</commit_message>
<xml_diff>
--- a/resources/schema.xlsx
+++ b/resources/schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dbecker/Developer/Otter-Pond/backend/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E230666F-008E-D043-B679-AC5FDAC428C1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9F81D8-08F2-E345-A3A0-945A2699339D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{0C720A25-C826-A445-B6B6-0EAA8761497C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>user</t>
   </si>
@@ -94,14 +94,31 @@
   </si>
   <si>
     <t>list_email_2</t>
+  </si>
+  <si>
+    <t>list_list_email_1</t>
+  </si>
+  <si>
+    <t>list_list_email_2</t>
+  </si>
+  <si>
+    <t>Other Attributes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -129,10 +146,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -451,26 +472,34 @@
   <dimension ref="B3:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="D3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
@@ -501,13 +530,13 @@
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="1"/>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
@@ -521,13 +550,13 @@
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9" s="1"/>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
@@ -571,10 +600,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="B10:B12"/>
+    <mergeCell ref="D3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Allow external senders for position emails
</commit_message>
<xml_diff>
--- a/resources/schema.xlsx
+++ b/resources/schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dbecker/Developer/Otter-Pond/backend/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9F81D8-08F2-E345-A3A0-945A2699339D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6749103-7440-D14C-B7F4-159BA8C98CFC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{0C720A25-C826-A445-B6B6-0EAA8761497C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>user</t>
   </si>
@@ -39,9 +39,6 @@
     <t>user_email_1</t>
   </si>
   <si>
-    <t>user_email_2</t>
-  </si>
-  <si>
     <t>first_name</t>
   </si>
   <si>
@@ -93,9 +90,6 @@
     <t>list_email_1</t>
   </si>
   <si>
-    <t>list_email_2</t>
-  </si>
-  <si>
     <t>list_list_email_1</t>
   </si>
   <si>
@@ -103,6 +97,12 @@
   </si>
   <si>
     <t>Other Attributes</t>
+  </si>
+  <si>
+    <t>role_id</t>
+  </si>
+  <si>
+    <t>allow_external</t>
   </si>
 </sst>
 </file>
@@ -148,10 +148,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -469,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A77775C-C977-0B41-B9E5-52FC31CBAEF5}">
-  <dimension ref="B3:I13"/>
+  <dimension ref="B3:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -486,14 +486,14 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -502,108 +502,96 @@
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
       </c>
       <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>5</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>6</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>7</v>
       </c>
-      <c r="I4" t="s">
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B5" s="2"/>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B6" s="2"/>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B8" s="2"/>
+      <c r="C8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="1"/>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="1"/>
-      <c r="C6" t="s">
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B8" s="1"/>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B9" s="1"/>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
         <v>14</v>
       </c>
-      <c r="E10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="1"/>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B10:B12"/>
     <mergeCell ref="D3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Auto add/remove from email lists on role change
</commit_message>
<xml_diff>
--- a/resources/schema.xlsx
+++ b/resources/schema.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dbecker/Developer/Otter-Pond/backend/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1344FE1B-B4E4-304D-8BE8-0C12950E2000}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4759B44C-FB9B-AD47-BC87-44D49F5D04BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{0C720A25-C826-A445-B6B6-0EAA8761497C}"/>
   </bookViews>
@@ -63,9 +63,6 @@
     <t>can_be_invited</t>
   </si>
   <si>
-    <t>joined_by_default</t>
-  </si>
-  <si>
     <t>subject_prefix</t>
   </si>
   <si>
@@ -181,6 +178,9 @@
   </si>
   <si>
     <t>end_date</t>
+  </si>
+  <si>
+    <t>default</t>
   </si>
 </sst>
 </file>
@@ -553,7 +553,7 @@
   <dimension ref="B3:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -568,13 +568,13 @@
   <sheetData>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -587,7 +587,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
         <v>1</v>
@@ -611,33 +611,33 @@
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" s="2"/>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="2"/>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>12</v>
       </c>
-      <c r="F7" t="s">
-        <v>13</v>
-      </c>
       <c r="G7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
@@ -652,7 +652,7 @@
         <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.2">
@@ -660,113 +660,113 @@
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
         <v>22</v>
       </c>
-      <c r="C11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>23</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>24</v>
-      </c>
-      <c r="F11" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
         <v>26</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>27</v>
-      </c>
-      <c r="D12" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
         <v>33</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>34</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>35</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>36</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>37</v>
-      </c>
-      <c r="G13" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B14" s="4"/>
       <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
         <v>39</v>
       </c>
-      <c r="D14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" t="s">
         <v>40</v>
-      </c>
-      <c r="F14" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
         <v>42</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" t="s">
         <v>43</v>
       </c>
-      <c r="D15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>44</v>
-      </c>
-      <c r="F15" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
         <v>46</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>47</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>48</v>
       </c>
-      <c r="E16" t="s">
-        <v>49</v>
-      </c>
       <c r="F16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Email list subscription update on role change
</commit_message>
<xml_diff>
--- a/resources/schema.xlsx
+++ b/resources/schema.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dbecker/Developer/Otter-Pond/backend/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1344FE1B-B4E4-304D-8BE8-0C12950E2000}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4759B44C-FB9B-AD47-BC87-44D49F5D04BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{0C720A25-C826-A445-B6B6-0EAA8761497C}"/>
   </bookViews>
@@ -63,9 +63,6 @@
     <t>can_be_invited</t>
   </si>
   <si>
-    <t>joined_by_default</t>
-  </si>
-  <si>
     <t>subject_prefix</t>
   </si>
   <si>
@@ -181,6 +178,9 @@
   </si>
   <si>
     <t>end_date</t>
+  </si>
+  <si>
+    <t>default</t>
   </si>
 </sst>
 </file>
@@ -553,7 +553,7 @@
   <dimension ref="B3:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -568,13 +568,13 @@
   <sheetData>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -587,7 +587,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
         <v>1</v>
@@ -611,33 +611,33 @@
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" s="2"/>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="2"/>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>12</v>
       </c>
-      <c r="F7" t="s">
-        <v>13</v>
-      </c>
       <c r="G7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
@@ -652,7 +652,7 @@
         <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.2">
@@ -660,113 +660,113 @@
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
         <v>22</v>
       </c>
-      <c r="C11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>23</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>24</v>
-      </c>
-      <c r="F11" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
         <v>26</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>27</v>
-      </c>
-      <c r="D12" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
         <v>33</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>34</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>35</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>36</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>37</v>
-      </c>
-      <c r="G13" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B14" s="4"/>
       <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
         <v>39</v>
       </c>
-      <c r="D14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" t="s">
         <v>40</v>
-      </c>
-      <c r="F14" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
         <v>42</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" t="s">
         <v>43</v>
       </c>
-      <c r="D15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>44</v>
-      </c>
-      <c r="F15" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
         <v>46</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>47</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>48</v>
       </c>
-      <c r="E16" t="s">
-        <v>49</v>
-      </c>
       <c r="F16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>